<commit_message>
Added times for graphsage
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathanielsprecher/Documents/REU_GNN/GraphSAGE_Benchmark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C95670-CEE2-6344-853D-FE7E61B599E5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D5165E-9EB7-3442-9E1B-D6AD153A72B2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="460" windowWidth="27640" windowHeight="15580" activeTab="3" xr2:uid="{126C32C7-39E5-4748-8F2C-16AAB677E73B}"/>
+    <workbookView xWindow="500" yWindow="460" windowWidth="27640" windowHeight="15580" xr2:uid="{126C32C7-39E5-4748-8F2C-16AAB677E73B}"/>
   </bookViews>
   <sheets>
     <sheet name="Ind_10n_4a" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="25">
   <si>
     <t>avg</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Avg Test_T</t>
+  </si>
+  <si>
+    <t>Avg Iter_T</t>
   </si>
 </sst>
 </file>
@@ -211,7 +217,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="57">
+  <borders count="59">
     <border>
       <left/>
       <right/>
@@ -943,12 +949,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
@@ -1077,6 +1109,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="57" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -15615,16 +15652,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>548407</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>294409</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>106217</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>215898</xdr:colOff>
+      <xdr:colOff>793172</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>138545</xdr:rowOff>
+      <xdr:rowOff>57728</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15653,16 +15690,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>519543</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>265544</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>71582</xdr:rowOff>
+      <xdr:rowOff>13855</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>187034</xdr:colOff>
+      <xdr:colOff>764307</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>138545</xdr:rowOff>
+      <xdr:rowOff>80818</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15691,16 +15728,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>819726</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>507999</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>25399</xdr:rowOff>
+      <xdr:rowOff>13853</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>484908</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>173181</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>92362</xdr:rowOff>
+      <xdr:rowOff>80816</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15730,15 +15767,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>51955</xdr:colOff>
+      <xdr:colOff>513774</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>94673</xdr:rowOff>
+      <xdr:rowOff>48490</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>550719</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>181265</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>127001</xdr:rowOff>
+      <xdr:rowOff>80818</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16379,8 +16416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88DA590C-06CB-1849-8E8B-D35982C91359}">
   <dimension ref="B2:L70"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="K44" sqref="K44"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -16822,6 +16859,45 @@
         <v>0.62485000000000002</v>
       </c>
     </row>
+    <row r="21" spans="2:12" ht="16" thickBot="1"/>
+    <row r="22" spans="2:12" ht="16" thickBot="1">
+      <c r="B22" s="112" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="113"/>
+      <c r="H22" s="112" t="s">
+        <v>9</v>
+      </c>
+      <c r="I22" s="116"/>
+    </row>
+    <row r="23" spans="2:12" ht="16" thickBot="1">
+      <c r="B23" s="104" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H23" s="104" t="s">
+        <v>23</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" ht="16" thickBot="1">
+      <c r="B24" s="114">
+        <v>2.1475900000000001</v>
+      </c>
+      <c r="C24" s="115">
+        <v>0.16064999999999999</v>
+      </c>
+      <c r="H24" s="114">
+        <v>6.0711599999999999</v>
+      </c>
+      <c r="I24" s="115">
+        <v>0.43429000000000001</v>
+      </c>
+    </row>
     <row r="31" spans="2:12" ht="16" thickBot="1"/>
     <row r="32" spans="2:12" ht="16" thickBot="1">
       <c r="B32" s="21" t="s">
@@ -18034,7 +18110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D99767B8-D82A-3D47-85CA-0BB753848A94}">
   <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="L2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
@@ -22095,8 +22171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82111682-450E-5C43-AB0C-8467E773F492}">
   <dimension ref="A2:M70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView topLeftCell="I1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>